<commit_message>
Clean up the output and stuff
</commit_message>
<xml_diff>
--- a/input_spreadsheet/test.xlsx
+++ b/input_spreadsheet/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="175">
   <si>
     <t>Guidelines for system hardening</t>
   </si>
@@ -117,6 +117,458 @@
   </si>
   <si>
     <t>Computer accounts that are not Microsoft AD DS domain controllers are not trusted for delegation to services.</t>
+  </si>
+  <si>
+    <t>Guidelines for personnel security</t>
+  </si>
+  <si>
+    <t>Access to systems and their resources</t>
+  </si>
+  <si>
+    <t>User identification</t>
+  </si>
+  <si>
+    <t>ISM-0414</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Aug-19</t>
+  </si>
+  <si>
+    <t>Personnel granted access to a system and its resources are uniquely identifiable.</t>
+  </si>
+  <si>
+    <t>ISM-0415</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>The use of shared user accounts is strictly controlled, and personnel using such accounts are uniquely identifiable.</t>
+  </si>
+  <si>
+    <t>ISM-1583</t>
+  </si>
+  <si>
+    <t>Aug-20</t>
+  </si>
+  <si>
+    <t>Personnel who are contractors are identified as such.</t>
+  </si>
+  <si>
+    <t>ISM-0420</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Dec-21</t>
+  </si>
+  <si>
+    <t>Where a system processes, stores or communicates AUSTEO, AGAO or REL data, personnel who are foreign nationals are identified as such, including by their specific nationality.</t>
+  </si>
+  <si>
+    <t>Unprivileged access to systems</t>
+  </si>
+  <si>
+    <t>ISM-0405</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Requests for unprivileged access to systems, applications and data repositories are validated when first requested.</t>
+  </si>
+  <si>
+    <t>ISM-1852</t>
+  </si>
+  <si>
+    <t>Jun-23</t>
+  </si>
+  <si>
+    <t>Unprivileged access to systems, applications and data repositories is limited to only what is required for users and services to undertake their duties.</t>
+  </si>
+  <si>
+    <t>ISM-1566</t>
+  </si>
+  <si>
+    <t>Dec-23</t>
+  </si>
+  <si>
+    <t>Use of unprivileged access is centrally logged.</t>
+  </si>
+  <si>
+    <t>Unprivileged access to systems by foreign nationals</t>
+  </si>
+  <si>
+    <t>ISM-0409</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Jun-22</t>
+  </si>
+  <si>
+    <t>Foreign nationals, including seconded foreign nationals, do not have access to systems that process, store or communicate AUSTEO or REL data unless effective controls are in place to ensure such data is not accessible to them.</t>
+  </si>
+  <si>
+    <t>ISM-0411</t>
+  </si>
+  <si>
+    <t>Foreign nationals, excluding seconded foreign nationals, do not have access to systems that process, store or communicate AGAO data unless effective controls are in place to ensure such data is not accessible to them.</t>
+  </si>
+  <si>
+    <t>Privileged access to systems</t>
+  </si>
+  <si>
+    <t>ISM-1507</t>
+  </si>
+  <si>
+    <t>Requests for privileged access to systems, applications and data repositories are validated when first requested.</t>
+  </si>
+  <si>
+    <t>ISM-1508</t>
+  </si>
+  <si>
+    <t>Privileged access to systems, applications and data repositories is limited to only what is required for users and services to undertake their duties.</t>
+  </si>
+  <si>
+    <t>ISM-1175</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Privileged user accounts (excluding those explicitly authorised to access online services) are prevented from accessing the internet, email and web services.</t>
+  </si>
+  <si>
+    <t>ISM-1883</t>
+  </si>
+  <si>
+    <t>Privileged user accounts explicitly authorised to access online services are strictly limited to only what is required for users and services to undertake their duties.</t>
+  </si>
+  <si>
+    <t>ISM-1649</t>
+  </si>
+  <si>
+    <t>Sep-21</t>
+  </si>
+  <si>
+    <t>Just-in-time administration is used for administering systems and applications.</t>
+  </si>
+  <si>
+    <t>ISM-0445</t>
+  </si>
+  <si>
+    <t>Privileged users are assigned a dedicated privileged user account to be used solely for duties requiring privileged access.</t>
+  </si>
+  <si>
+    <t>ISM-1263</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Unique privileged user accounts are used for administering individual server applications.</t>
+  </si>
+  <si>
+    <t>ISM-1509</t>
+  </si>
+  <si>
+    <t>Privileged access events are centrally logged.</t>
+  </si>
+  <si>
+    <t>ISM-1650</t>
+  </si>
+  <si>
+    <t>Privileged user account and security group management events are centrally logged.</t>
+  </si>
+  <si>
+    <t>Privileged access to systems by foreign nationals</t>
+  </si>
+  <si>
+    <t>ISM-0446</t>
+  </si>
+  <si>
+    <t>Jun-21</t>
+  </si>
+  <si>
+    <t>Foreign nationals, including seconded foreign nationals, do not have privileged access to systems that process, store or communicate AUSTEO or REL data.</t>
+  </si>
+  <si>
+    <t>ISM-0447</t>
+  </si>
+  <si>
+    <t>Foreign nationals, excluding seconded foreign nationals, do not have privileged access to systems that process, store or communicate AGAO data.</t>
+  </si>
+  <si>
+    <t>Suspension of access to systems</t>
+  </si>
+  <si>
+    <t>ISM-0430</t>
+  </si>
+  <si>
+    <t>Sep-19</t>
+  </si>
+  <si>
+    <t>Access to systems, applications and data repositories is removed or suspended on the same day personnel no longer have a legitimate requirement for access.</t>
+  </si>
+  <si>
+    <t>ISM-1591</t>
+  </si>
+  <si>
+    <t>Access to systems, applications and data repositories is removed or suspended as soon as practicable when personnel are detected undertaking malicious activities.</t>
+  </si>
+  <si>
+    <t>ISM-1404</t>
+  </si>
+  <si>
+    <t>Unprivileged access to systems and applications is disabled after 45 days of inactivity.</t>
+  </si>
+  <si>
+    <t>ISM-1648</t>
+  </si>
+  <si>
+    <t>Privileged access to systems and applications is disabled after 45 days of inactivity.</t>
+  </si>
+  <si>
+    <t>ISM-1716</t>
+  </si>
+  <si>
+    <t>Access to data repositories is disabled after 45 days of inactivity.</t>
+  </si>
+  <si>
+    <t>ISM-1647</t>
+  </si>
+  <si>
+    <t>Privileged access to systems, applications and data repositories is disabled after 12 months unless revalidated.</t>
+  </si>
+  <si>
+    <t>Recording authorisation for personnel to access systems</t>
+  </si>
+  <si>
+    <t>ISM-0407</t>
+  </si>
+  <si>
+    <t>Sep-23</t>
+  </si>
+  <si>
+    <t>A secure record is maintained for the life of each system covering the following for each user:
+• their user identification
+• their signed agreement to abide by usage policies for the system and its resources
+• who provided authorisation for their access
+• when their access was granted
+• the level of access that they were granted
+• when their access, and their level of access, was last reviewed
+• when their level of access was changed, and to what extent (if applicable)
+• when their access was withdrawn (if applicable).</t>
+  </si>
+  <si>
+    <t>Temporary access to systems</t>
+  </si>
+  <si>
+    <t>ISM-0441</t>
+  </si>
+  <si>
+    <t>When personnel are granted temporary access to a system, effective controls are put in place to restrict their access to only data required for them to undertake their duties.</t>
+  </si>
+  <si>
+    <t>ISM-0443</t>
+  </si>
+  <si>
+    <t>Sep-18</t>
+  </si>
+  <si>
+    <t>Temporary access is not granted to systems that process, store or communicate caveated or sensitive compartmented information.</t>
+  </si>
+  <si>
+    <t>Emergency access to systems</t>
+  </si>
+  <si>
+    <t>ISM-1610</t>
+  </si>
+  <si>
+    <t>A method of emergency access to systems is documented and tested at least once when initially implemented and each time fundamental information technology infrastructure changes occur.</t>
+  </si>
+  <si>
+    <t>ISM-1611</t>
+  </si>
+  <si>
+    <t>Break glass accounts are only used when normal authentication processes cannot be used.</t>
+  </si>
+  <si>
+    <t>ISM-1612</t>
+  </si>
+  <si>
+    <t>Break glass accounts are only used for specific authorised activities.</t>
+  </si>
+  <si>
+    <t>ISM-1614</t>
+  </si>
+  <si>
+    <t>Break glass account credentials are changed by the account custodian after they are accessed by any other party.</t>
+  </si>
+  <si>
+    <t>ISM-1615</t>
+  </si>
+  <si>
+    <t>Break glass accounts are tested after credentials are changed.</t>
+  </si>
+  <si>
+    <t>ISM-1613</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Use of break glass accounts is centrally logged.</t>
+  </si>
+  <si>
+    <t>Control of Australian systems</t>
+  </si>
+  <si>
+    <t>ISM-0078</t>
+  </si>
+  <si>
+    <t>Systems processing, storing or communicating AUSTEO or AGAO data remain at all times under the control of an Australian national working for or on behalf of the Australian Government.</t>
+  </si>
+  <si>
+    <t>ISM-0854</t>
+  </si>
+  <si>
+    <t>AUSTEO and AGAO data can only be accessed from systems under the sole control of the Australian Government that are located within facilities authorised by the Australian Government.</t>
+  </si>
+  <si>
+    <t>Guidelines for communications infrastructure</t>
+  </si>
+  <si>
+    <t>Cabling infrastructure</t>
+  </si>
+  <si>
+    <t>Cabling infrastructure standards</t>
+  </si>
+  <si>
+    <t>ISM-0181</t>
+  </si>
+  <si>
+    <t>Mar-21</t>
+  </si>
+  <si>
+    <t>Cabling infrastructure is installed in accordance with relevant Australian Standards, as directed by the Australian Communications and Media Authority.</t>
+  </si>
+  <si>
+    <t>Use of fibre-optic cables</t>
+  </si>
+  <si>
+    <t>ISM-1111</t>
+  </si>
+  <si>
+    <t>Fibre-optic cables are used for cabling infrastructure instead of copper cables.</t>
+  </si>
+  <si>
+    <t>Cable register</t>
+  </si>
+  <si>
+    <t>ISM-0211</t>
+  </si>
+  <si>
+    <t>Dec-22</t>
+  </si>
+  <si>
+    <t>A cable register is developed, implemented, maintained and verified on a regular basis.</t>
+  </si>
+  <si>
+    <t>ISM-0208</t>
+  </si>
+  <si>
+    <t>A cable register contains the following for each cable:
+• cable identifier
+• cable colour
+• sensitivity/classification
+• source
+• destination
+• location
+• seal numbers (if applicable).</t>
+  </si>
+  <si>
+    <t>Floor plan diagrams</t>
+  </si>
+  <si>
+    <t>ISM-1645</t>
+  </si>
+  <si>
+    <t>Floor plan diagrams are developed, implemented, maintained and verified on a regular basis.</t>
+  </si>
+  <si>
+    <t>ISM-1646</t>
+  </si>
+  <si>
+    <t>Floor plan diagrams contain the following:
+• cable paths (including ingress and egress points between floors)
+• cable reticulation system and conduit paths
+• floor concentration boxes
+• wall outlet boxes
+• network cabinets.</t>
+  </si>
+  <si>
+    <t>Cable labelling processes and procedures</t>
+  </si>
+  <si>
+    <t>ISM-0206</t>
+  </si>
+  <si>
+    <t>Cable labelling processes, and supporting cable labelling procedures, are developed, implemented and maintained.</t>
+  </si>
+  <si>
+    <t>Labelling cables</t>
+  </si>
+  <si>
+    <t>ISM-1096</t>
+  </si>
+  <si>
+    <t>Oct-19</t>
+  </si>
+  <si>
+    <t>Cables are labelled at each end with sufficient source and destination details to enable the physical identification and inspection of the cable.</t>
+  </si>
+  <si>
+    <t>Labelling building management cables</t>
+  </si>
+  <si>
+    <t>ISM-1639</t>
+  </si>
+  <si>
+    <t>Building management cables are labelled with their purpose in black writing on a yellow background, with a minimum size of 2.5 cm x 1 cm, and attached at five-metre intervals.</t>
+  </si>
+  <si>
+    <t>Labelling cables for foreign systems in Australian facilities</t>
+  </si>
+  <si>
+    <t>ISM-1640</t>
+  </si>
+  <si>
+    <t>Cables for foreign systems installed in Australian facilities are labelled at inspection points.</t>
+  </si>
+  <si>
+    <t>Cable colours</t>
+  </si>
+  <si>
+    <t>ISM-1820</t>
+  </si>
+  <si>
+    <t>Cables for individual systems use a consistent colour.</t>
+  </si>
+  <si>
+    <t>ISM-0926</t>
+  </si>
+  <si>
+    <t>Dec-24</t>
+  </si>
+  <si>
+    <t>Non-classified, OFFICIAL: Sensitive and PROTECTED cables are coloured neither salmon pink nor red.</t>
   </si>
 </sst>
 </file>
@@ -468,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,6 +1445,2309 @@
         <v>30</v>
       </c>
     </row>
+    <row r="12" spans="1:15" ht="138" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="207" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="289.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="207" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="276" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="386.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="372.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="262.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="276" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="303.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="151.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="207" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="262.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="262.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="289.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="151.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="138" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="193.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="303.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="248.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="358.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="207" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="317.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="262.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="138" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="345" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="400.2" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="207" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="234.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="276" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O60" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>